<commit_message>
-ExcelSuiteParser: minor updates and clean up -Added Apache License 2.0, changes.txt -Added tests to ExcelSuiteParserTest2
</commit_message>
<xml_diff>
--- a/src/test/tests.xlsx
+++ b/src/test/tests.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2910" windowWidth="10485" windowHeight="3225"/>
+    <workbookView xWindow="0" yWindow="2910" windowWidth="10485" windowHeight="3225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.GoogleSearch.FF" sheetId="6" r:id="rId1"/>
     <sheet name="2.GoogleSearch.IE" sheetId="5" r:id="rId2"/>
+    <sheet name="InvalidSuite" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="NamedRange" localSheetId="0">'1.GoogleSearch.FF'!#REF!</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Test Name</t>
   </si>
@@ -92,6 +93,12 @@
     <t>testUrl=http://www.google.com
 browser=internet explorer
 hubUrl=http://localhost:4444/wd/hub</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -576,7 +583,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -634,6 +641,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -679,7 +699,33 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF4F81BD"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF4F81BD"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF4F81BD"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF4F81BD"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF4F81BD"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border outline="0">
         <left style="thin">
@@ -703,36 +749,13 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF4F81BD"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF4F81BD"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF4F81BD"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF4F81BD"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF4F81BD"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A8:F10" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A8:F10" headerRowBorderDxfId="1" tableBorderDxfId="2">
   <autoFilter ref="A8:F10"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Id" totalsRowLabel="Total"/>
@@ -747,10 +770,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:F10" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A8:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B8:G21" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B8:G21"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="Total"/>
+    <tableColumn id="1" name="Id" totalsRowLabel="Total" dataDxfId="0"/>
     <tableColumn id="2" name="Application"/>
     <tableColumn id="3" name="Test Name"/>
     <tableColumn id="4" name="Test Description"/>
@@ -1051,9 +1074,9 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1196,11 +1219,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1209,17 +1232,18 @@
     <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="35.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2"/>
       <c r="B2" t="s">
         <v>9</v>
@@ -1228,7 +1252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3"/>
       <c r="B3" t="s">
         <v>10</v>
@@ -1237,7 +1261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="38.25">
+    <row r="4" spans="1:7" ht="38.25">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>11</v>
@@ -1246,86 +1270,150 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7"/>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1"/>
       <c r="B7"/>
       <c r="C7"/>
-    </row>
-    <row r="8" spans="1:6" ht="13.5" thickBot="1">
-      <c r="A8" s="12" t="s">
+      <c r="D7"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="7">
+    <row r="9" spans="1:7">
+      <c r="A9" s="1"/>
+      <c r="B9" s="21">
         <v>2.1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="17">
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="22">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11"/>
-      <c r="B11"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1"/>
+      <c r="B11" s="23">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="C11"/>
+      <c r="D11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1"/>
+      <c r="B12" s="22">
+        <v>2.4</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="23">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="22">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="4"/>
+      <c r="B20" s="25"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="24"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -1336,4 +1424,34 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>